<commit_message>
Adding Feature Files to the Git
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ShareWebCopy_Guvi_BestBuy\ShareWebCopy\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ShareWebCopy_Guvi_BestBuy\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C0C60A-F18E-4967-A4C9-D8ECC776A5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600ED186-C8B5-451E-B427-7B2B07950578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,12 +172,6 @@
     <t>VGMENUS</t>
   </si>
   <si>
-    <t>Nintendo;PlayStation;Xbox;PC Gaming;Virtual Reality;Gaming Accessories;Digital Gaming;Handheld Gaming;Deals &amp; Outlet</t>
-  </si>
-  <si>
-    <t>Retro Gaming &amp; Arcade;All Video Games;Nintendo Switch 2 Notifications;ROG Ally Gaming Handheld;Video Game Announcements</t>
-  </si>
-  <si>
     <t>CCDSUBMENUS</t>
   </si>
   <si>
@@ -301,15 +295,9 @@
     <t>Electric Bikes;Electric Scooters;Kids' Scooters &amp; Ride-Ons;Safety Gear &amp; Accessories;Deals;Services &amp; Support</t>
   </si>
   <si>
-    <t>Featured Gift Ideas;New Releases;Top-Rated Tech;Discover &amp; Learn Blog;Winter Shop</t>
-  </si>
-  <si>
     <t>FTAPPAGEURL</t>
   </si>
   <si>
-    <t>identity/signin;shipping-delivery-store-pickup;return-exchange-policy;price-match-guarantee;product-recalls;trade-in;gift-cards;financing-rewards;identity/signin;progressive-leasing;financing-rewards;support;shopping;services;appointmentfinder;electronics/services;recycling;contact-us;best-buy-membership;identity/signin;loyalty/catalog;marketplace;bestbuyads.com;identity/signin;loyalty/catalog;marketplace;www.bestbuyads.com;best-buy-affiliate-program;bestbuyhealth.com;bestbuy-education;bestbuy-business;partner-plus;developer.bestbuy.com;corporate.bestbuy.com;jobs.bestbuy.com;corporate.bestbuy.com;corporate.bestbuy.com</t>
-  </si>
-  <si>
     <t>support;identity/signin;shipping-delivery-store-pickup;return-exchange-policy</t>
   </si>
   <si>
@@ -386,6 +374,18 @@
   </si>
   <si>
     <t>bhaanu;reaka;1201 North Muldoon Street;Anchorage;AK;99504;Bhaanu@123456</t>
+  </si>
+  <si>
+    <t>Nintendo;Xbox;PlayStation;PC Gaming;Virtual Reality;Gaming Accessories;Digital Gaming;Handheld Gaming;Deals &amp; Outlet</t>
+  </si>
+  <si>
+    <t>identity/signin;shipping-delivery-store-pickup;return-exchange-policy;price-match-guarantee;product-recalls;trade-in;gift-cards;financing-rewards;identity/signin;progressive-leasing;financing-rewards;support;shopping;services;appointmentfinder;electronics/services;recycling;contact-us;best-buy-membership;identity/signin;loyalty/catalog;marketplace;bestbuyads.com;identity/signin;loyalty/catalog;marketplace;www.bestbuyads.com;best-buy-affiliate-program;bestbuyhealth.com;bestbuy-education;bestbuy-business;partner-plus;corporate.bestbuy.com;jobs.bestbuy.com;corporate.bestbuy.com;corporate.bestbuy.com</t>
+  </si>
+  <si>
+    <t>Featured Gift Ideas;New Releases;Top-Rated Tech;Discover &amp; Learn Blog;Spring Shop</t>
+  </si>
+  <si>
+    <t>Retro Gaming &amp; Arcade;All Video Games;Nintendo Switch 2;ROG Ally Gaming Handheld;Video Game Announcements</t>
   </si>
 </sst>
 </file>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W825"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="16" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="2"/>
@@ -1485,7 +1485,7 @@
         <v>48</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="2"/>
@@ -1514,7 +1514,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="2"/>
@@ -1540,10 +1540,10 @@
     </row>
     <row r="27" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="28" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="2"/>
@@ -1598,10 +1598,10 @@
     </row>
     <row r="29" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="2"/>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="30" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="2"/>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="31" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="32" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="2"/>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="33" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="2"/>
@@ -1743,10 +1743,10 @@
     </row>
     <row r="34" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="2"/>
@@ -1772,10 +1772,10 @@
     </row>
     <row r="35" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="2"/>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="36" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="2"/>
@@ -1830,10 +1830,10 @@
     </row>
     <row r="37" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="2"/>
@@ -1859,10 +1859,10 @@
     </row>
     <row r="38" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A38" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="2"/>
@@ -1888,10 +1888,10 @@
     </row>
     <row r="39" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A39" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="2"/>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="40" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A40" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="2"/>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="41" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="2"/>
@@ -1975,10 +1975,10 @@
     </row>
     <row r="42" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="2"/>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="43" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="2"/>
@@ -2033,10 +2033,10 @@
     </row>
     <row r="44" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="2"/>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="45" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="46" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="2"/>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="47" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A47" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="2"/>
@@ -2149,10 +2149,10 @@
     </row>
     <row r="48" spans="1:23" ht="67.5" customHeight="1" thickBot="1">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="2"/>
@@ -2178,10 +2178,10 @@
     </row>
     <row r="49" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A49" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="2"/>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="50" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="2"/>
@@ -2236,10 +2236,10 @@
     </row>
     <row r="51" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="2"/>
@@ -2265,10 +2265,10 @@
     </row>
     <row r="52" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="2"/>
@@ -2294,10 +2294,10 @@
     </row>
     <row r="53" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="2"/>
@@ -2323,10 +2323,10 @@
     </row>
     <row r="54" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="2"/>
@@ -2352,10 +2352,10 @@
     </row>
     <row r="55" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A55" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="2"/>
@@ -2381,10 +2381,10 @@
     </row>
     <row r="56" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="2"/>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="57" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A57" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="2"/>
@@ -2439,10 +2439,10 @@
     </row>
     <row r="58" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A58" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="2"/>
@@ -2468,10 +2468,10 @@
     </row>
     <row r="59" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A59" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C59" s="12"/>
       <c r="D59" s="2"/>
@@ -2497,10 +2497,10 @@
     </row>
     <row r="60" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A60" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="2"/>

</xml_diff>

<commit_message>
Adding iml files to git
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ShareWebCopy_Guvi_BestBuy\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600ED186-C8B5-451E-B427-7B2B07950578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56024F-1F63-4964-8547-7D240342898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>KEY</t>
   </si>
@@ -28,16 +28,10 @@
     <t>QA</t>
   </si>
   <si>
-    <t>PROD</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
     <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>https://v2web.mmhnz.cloud/</t>
   </si>
   <si>
     <t>https://www.bestbuy.com/</t>
@@ -392,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,12 +420,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="9.8000000000000007"/>
       <color rgb="FF297BDE"/>
@@ -447,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -471,36 +459,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
@@ -516,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -529,22 +487,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -766,30 +715,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W825"/>
+  <dimension ref="A1:V825"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="36.7265625" customWidth="1"/>
     <col min="2" max="2" width="161.453125" customWidth="1"/>
-    <col min="3" max="3" width="161.1796875" customWidth="1"/>
-    <col min="4" max="23" width="8.81640625" customWidth="1"/>
+    <col min="3" max="22" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="13.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="1" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -809,18 +755,15 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="2" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -840,16 +783,15 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-    </row>
-    <row r="3" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="3" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -869,16 +811,15 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="4" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -898,16 +839,15 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="5" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -927,16 +867,15 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="6" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -956,16 +895,15 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="7" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -985,16 +923,15 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="8" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1014,16 +951,15 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="9" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1043,16 +979,15 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="10" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1072,16 +1007,15 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="11" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1101,16 +1035,15 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" ht="63.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="12" spans="1:22" ht="63.5" customHeight="1" thickBot="1">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1130,16 +1063,15 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="13" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="12"/>
+        <v>24</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1159,16 +1091,15 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="14" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1188,16 +1119,15 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="15" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1217,16 +1147,15 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="16" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1246,16 +1175,15 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="17" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1275,16 +1203,15 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="18" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1304,16 +1231,15 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="19" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1333,16 +1259,15 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="20" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1362,16 +1287,15 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="21" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="B21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1391,16 +1315,15 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="22" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1420,16 +1343,15 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="23" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1449,16 +1371,15 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-    </row>
-    <row r="24" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="24" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1478,16 +1399,15 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-    </row>
-    <row r="25" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="25" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1507,16 +1427,15 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-    </row>
-    <row r="26" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="26" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1536,16 +1455,15 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-    </row>
-    <row r="27" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="27" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -1565,16 +1483,15 @@
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-    </row>
-    <row r="28" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="28" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1594,16 +1511,15 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-    </row>
-    <row r="29" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="29" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1623,16 +1539,15 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-    </row>
-    <row r="30" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="30" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1652,16 +1567,15 @@
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-    </row>
-    <row r="31" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="31" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1681,16 +1595,15 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-    </row>
-    <row r="32" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="32" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1710,16 +1623,15 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-    </row>
-    <row r="33" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="33" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1739,16 +1651,15 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-    </row>
-    <row r="34" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="34" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1768,16 +1679,15 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-    </row>
-    <row r="35" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="35" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1797,16 +1707,15 @@
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-    </row>
-    <row r="36" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="36" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1826,16 +1735,15 @@
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-    </row>
-    <row r="37" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="37" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1855,16 +1763,15 @@
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
-    </row>
-    <row r="38" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="38" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1884,16 +1791,15 @@
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-    </row>
-    <row r="39" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="39" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -1913,16 +1819,15 @@
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-    </row>
-    <row r="40" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="40" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="12"/>
+        <v>71</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1942,16 +1847,15 @@
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-    </row>
-    <row r="41" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="41" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1971,16 +1875,15 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
-    </row>
-    <row r="42" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="42" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2000,16 +1903,15 @@
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-    </row>
-    <row r="43" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="43" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2029,16 +1931,15 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
-    </row>
-    <row r="44" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="44" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="12"/>
+        <v>80</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -2058,16 +1959,15 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-    </row>
-    <row r="45" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="45" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2087,16 +1987,15 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-    </row>
-    <row r="46" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="46" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2116,16 +2015,15 @@
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-    </row>
-    <row r="47" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="47" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="12"/>
+        <v>91</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -2145,16 +2043,15 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
-    </row>
-    <row r="48" spans="1:23" ht="67.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="48" spans="1:22" ht="67.5" customHeight="1" thickBot="1">
       <c r="A48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -2174,16 +2071,15 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-    </row>
-    <row r="49" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="49" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -2203,16 +2099,15 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-    </row>
-    <row r="50" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="50" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A50" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -2232,16 +2127,15 @@
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
-    </row>
-    <row r="51" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="51" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A51" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C51" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -2261,16 +2155,15 @@
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
-    </row>
-    <row r="52" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="52" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A52" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="12"/>
+        <v>96</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -2290,16 +2183,15 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
-      <c r="W52" s="2"/>
-    </row>
-    <row r="53" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="53" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A53" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -2319,16 +2211,15 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
-      <c r="W53" s="2"/>
-    </row>
-    <row r="54" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="54" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A54" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C54" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -2348,16 +2239,15 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
-    </row>
-    <row r="55" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="55" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A55" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -2377,16 +2267,15 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
-    </row>
-    <row r="56" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="56" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A56" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C56" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -2406,16 +2295,15 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
-    </row>
-    <row r="57" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="57" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A57" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C57" s="12"/>
+        <v>103</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -2435,16 +2323,15 @@
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
-    </row>
-    <row r="58" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="58" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58" s="12"/>
+      <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -2464,16 +2351,15 @@
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
-      <c r="W58" s="2"/>
-    </row>
-    <row r="59" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="59" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A59" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -2493,16 +2379,15 @@
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
-      <c r="W59" s="2"/>
-    </row>
-    <row r="60" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="60" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A60" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -2522,12 +2407,11 @@
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
-      <c r="W60" s="2"/>
-    </row>
-    <row r="61" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
+    </row>
+    <row r="61" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -2547,12 +2431,11 @@
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
-      <c r="W61" s="2"/>
-    </row>
-    <row r="62" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
+    </row>
+    <row r="62" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -2572,12 +2455,11 @@
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
-      <c r="W62" s="2"/>
-    </row>
-    <row r="63" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
+    </row>
+    <row r="63" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -2597,12 +2479,11 @@
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
-      <c r="W63" s="2"/>
-    </row>
-    <row r="64" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
+    </row>
+    <row r="64" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -2622,12 +2503,11 @@
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
-      <c r="W64" s="2"/>
-    </row>
-    <row r="65" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
+    </row>
+    <row r="65" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -2647,12 +2527,11 @@
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
-      <c r="W65" s="2"/>
-    </row>
-    <row r="66" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="12"/>
+    </row>
+    <row r="66" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -2672,12 +2551,11 @@
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
-      <c r="W66" s="2"/>
-    </row>
-    <row r="67" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
+    </row>
+    <row r="67" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -2697,12 +2575,11 @@
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
-      <c r="W67" s="2"/>
-    </row>
-    <row r="68" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="12"/>
+    </row>
+    <row r="68" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -2722,12 +2599,11 @@
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
-      <c r="W68" s="2"/>
-    </row>
-    <row r="69" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A69" s="13"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
+    </row>
+    <row r="69" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A69" s="10"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2747,12 +2623,11 @@
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
-      <c r="W69" s="2"/>
-    </row>
-    <row r="70" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="70" spans="1:22" ht="13.5" customHeight="1">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -2772,12 +2647,11 @@
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
-      <c r="W70" s="2"/>
-    </row>
-    <row r="71" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="71" spans="1:22" ht="13.5" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
+      <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2797,12 +2671,11 @@
       <c r="T71" s="2"/>
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
-      <c r="W71" s="2"/>
-    </row>
-    <row r="72" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="72" spans="1:22" ht="13.5" customHeight="1">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
+      <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2822,12 +2695,11 @@
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
-      <c r="W72" s="2"/>
-    </row>
-    <row r="73" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="73" spans="1:22" ht="13.5" customHeight="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
+      <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2847,12 +2719,11 @@
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
-      <c r="W73" s="2"/>
-    </row>
-    <row r="74" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="74" spans="1:22" ht="13.5" customHeight="1">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
+      <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2872,12 +2743,11 @@
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
-      <c r="W74" s="2"/>
-    </row>
-    <row r="75" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="75" spans="1:22" ht="13.5" customHeight="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
+      <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2897,12 +2767,11 @@
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
-      <c r="W75" s="2"/>
-    </row>
-    <row r="76" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="76" spans="1:22" ht="13.5" customHeight="1">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
+      <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2922,12 +2791,11 @@
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
-      <c r="W76" s="2"/>
-    </row>
-    <row r="77" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="77" spans="1:22" ht="13.5" customHeight="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
+      <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2947,12 +2815,11 @@
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
-      <c r="W77" s="2"/>
-    </row>
-    <row r="78" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="78" spans="1:22" ht="13.5" customHeight="1">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
+      <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2972,12 +2839,11 @@
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
-      <c r="W78" s="2"/>
-    </row>
-    <row r="79" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="79" spans="1:22" ht="13.5" customHeight="1">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
+      <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -2997,12 +2863,11 @@
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
-      <c r="W79" s="2"/>
-    </row>
-    <row r="80" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="80" spans="1:22" ht="13.5" customHeight="1">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
+      <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -3022,12 +2887,11 @@
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
-      <c r="W80" s="2"/>
-    </row>
-    <row r="81" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="81" spans="1:22" ht="13.5" customHeight="1">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
+      <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -3047,12 +2911,11 @@
       <c r="T81" s="2"/>
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-    </row>
-    <row r="82" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="82" spans="1:22" ht="13.5" customHeight="1">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
+      <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -3072,12 +2935,11 @@
       <c r="T82" s="2"/>
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
-      <c r="W82" s="2"/>
-    </row>
-    <row r="83" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="83" spans="1:22" ht="13.5" customHeight="1">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
+      <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
@@ -3097,12 +2959,11 @@
       <c r="T83" s="2"/>
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
-      <c r="W83" s="2"/>
-    </row>
-    <row r="84" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="84" spans="1:22" ht="13.5" customHeight="1">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
+      <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -3122,12 +2983,11 @@
       <c r="T84" s="2"/>
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
-      <c r="W84" s="2"/>
-    </row>
-    <row r="85" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="85" spans="1:22" ht="13.5" customHeight="1">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
+      <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
@@ -3147,12 +3007,11 @@
       <c r="T85" s="2"/>
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
-      <c r="W85" s="2"/>
-    </row>
-    <row r="86" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="86" spans="1:22" ht="13.5" customHeight="1">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
+      <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -3172,12 +3031,11 @@
       <c r="T86" s="2"/>
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
-      <c r="W86" s="2"/>
-    </row>
-    <row r="87" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="87" spans="1:22" ht="13.5" customHeight="1">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
+      <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -3197,12 +3055,11 @@
       <c r="T87" s="2"/>
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
-      <c r="W87" s="2"/>
-    </row>
-    <row r="88" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="88" spans="1:22" ht="13.5" customHeight="1">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
+      <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -3222,12 +3079,11 @@
       <c r="T88" s="2"/>
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
-      <c r="W88" s="2"/>
-    </row>
-    <row r="89" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="89" spans="1:22" ht="13.5" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
+      <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -3247,12 +3103,11 @@
       <c r="T89" s="2"/>
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
-      <c r="W89" s="2"/>
-    </row>
-    <row r="90" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="90" spans="1:22" ht="13.5" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
+      <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -3272,12 +3127,11 @@
       <c r="T90" s="2"/>
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
-      <c r="W90" s="2"/>
-    </row>
-    <row r="91" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="91" spans="1:22" ht="13.5" customHeight="1">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
+      <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -3297,12 +3151,11 @@
       <c r="T91" s="2"/>
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
-      <c r="W91" s="2"/>
-    </row>
-    <row r="92" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="92" spans="1:22" ht="13.5" customHeight="1">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
+      <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -3322,12 +3175,11 @@
       <c r="T92" s="2"/>
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
-      <c r="W92" s="2"/>
-    </row>
-    <row r="93" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="93" spans="1:22" ht="13.5" customHeight="1">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
+      <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -3347,12 +3199,11 @@
       <c r="T93" s="2"/>
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
-      <c r="W93" s="2"/>
-    </row>
-    <row r="94" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="94" spans="1:22" ht="13.5" customHeight="1">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
+      <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -3372,12 +3223,11 @@
       <c r="T94" s="2"/>
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
-      <c r="W94" s="2"/>
-    </row>
-    <row r="95" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="95" spans="1:22" ht="13.5" customHeight="1">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
+      <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -3397,12 +3247,11 @@
       <c r="T95" s="2"/>
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
-      <c r="W95" s="2"/>
-    </row>
-    <row r="96" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="96" spans="1:22" ht="13.5" customHeight="1">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
+      <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -3422,12 +3271,11 @@
       <c r="T96" s="2"/>
       <c r="U96" s="2"/>
       <c r="V96" s="2"/>
-      <c r="W96" s="2"/>
-    </row>
-    <row r="97" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="97" spans="1:22" ht="13.5" customHeight="1">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
+      <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -3447,12 +3295,11 @@
       <c r="T97" s="2"/>
       <c r="U97" s="2"/>
       <c r="V97" s="2"/>
-      <c r="W97" s="2"/>
-    </row>
-    <row r="98" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="98" spans="1:22" ht="13.5" customHeight="1">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
+      <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -3472,12 +3319,11 @@
       <c r="T98" s="2"/>
       <c r="U98" s="2"/>
       <c r="V98" s="2"/>
-      <c r="W98" s="2"/>
-    </row>
-    <row r="99" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="99" spans="1:22" ht="13.5" customHeight="1">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
+      <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -3497,12 +3343,11 @@
       <c r="T99" s="2"/>
       <c r="U99" s="2"/>
       <c r="V99" s="2"/>
-      <c r="W99" s="2"/>
-    </row>
-    <row r="100" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="100" spans="1:22" ht="13.5" customHeight="1">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
+      <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -3522,12 +3367,11 @@
       <c r="T100" s="2"/>
       <c r="U100" s="2"/>
       <c r="V100" s="2"/>
-      <c r="W100" s="2"/>
-    </row>
-    <row r="101" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="101" spans="1:22" ht="13.5" customHeight="1">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
+      <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -3547,12 +3391,11 @@
       <c r="T101" s="2"/>
       <c r="U101" s="2"/>
       <c r="V101" s="2"/>
-      <c r="W101" s="2"/>
-    </row>
-    <row r="102" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="102" spans="1:22" ht="13.5" customHeight="1">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
+      <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -3572,12 +3415,11 @@
       <c r="T102" s="2"/>
       <c r="U102" s="2"/>
       <c r="V102" s="2"/>
-      <c r="W102" s="2"/>
-    </row>
-    <row r="103" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="103" spans="1:22" ht="13.5" customHeight="1">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
+      <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -3597,12 +3439,11 @@
       <c r="T103" s="2"/>
       <c r="U103" s="2"/>
       <c r="V103" s="2"/>
-      <c r="W103" s="2"/>
-    </row>
-    <row r="104" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="104" spans="1:22" ht="13.5" customHeight="1">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
+      <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -3622,12 +3463,11 @@
       <c r="T104" s="2"/>
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
-      <c r="W104" s="2"/>
-    </row>
-    <row r="105" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="105" spans="1:22" ht="13.5" customHeight="1">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
+      <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -3647,12 +3487,11 @@
       <c r="T105" s="2"/>
       <c r="U105" s="2"/>
       <c r="V105" s="2"/>
-      <c r="W105" s="2"/>
-    </row>
-    <row r="106" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="106" spans="1:22" ht="13.5" customHeight="1">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
+      <c r="C106" s="2"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -3672,12 +3511,11 @@
       <c r="T106" s="2"/>
       <c r="U106" s="2"/>
       <c r="V106" s="2"/>
-      <c r="W106" s="2"/>
-    </row>
-    <row r="107" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="107" spans="1:22" ht="13.5" customHeight="1">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
+      <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -3697,12 +3535,11 @@
       <c r="T107" s="2"/>
       <c r="U107" s="2"/>
       <c r="V107" s="2"/>
-      <c r="W107" s="2"/>
-    </row>
-    <row r="108" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="108" spans="1:22" ht="13.5" customHeight="1">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
+      <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -3722,12 +3559,11 @@
       <c r="T108" s="2"/>
       <c r="U108" s="2"/>
       <c r="V108" s="2"/>
-      <c r="W108" s="2"/>
-    </row>
-    <row r="109" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="109" spans="1:22" ht="13.5" customHeight="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
+      <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -3747,12 +3583,11 @@
       <c r="T109" s="2"/>
       <c r="U109" s="2"/>
       <c r="V109" s="2"/>
-      <c r="W109" s="2"/>
-    </row>
-    <row r="110" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="110" spans="1:22" ht="13.5" customHeight="1">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
+      <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -3772,12 +3607,11 @@
       <c r="T110" s="2"/>
       <c r="U110" s="2"/>
       <c r="V110" s="2"/>
-      <c r="W110" s="2"/>
-    </row>
-    <row r="111" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="111" spans="1:22" ht="13.5" customHeight="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
+      <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -3797,12 +3631,11 @@
       <c r="T111" s="2"/>
       <c r="U111" s="2"/>
       <c r="V111" s="2"/>
-      <c r="W111" s="2"/>
-    </row>
-    <row r="112" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="112" spans="1:22" ht="13.5" customHeight="1">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
+      <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -3822,12 +3655,11 @@
       <c r="T112" s="2"/>
       <c r="U112" s="2"/>
       <c r="V112" s="2"/>
-      <c r="W112" s="2"/>
-    </row>
-    <row r="113" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="113" spans="1:22" ht="13.5" customHeight="1">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
+      <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -3847,12 +3679,11 @@
       <c r="T113" s="2"/>
       <c r="U113" s="2"/>
       <c r="V113" s="2"/>
-      <c r="W113" s="2"/>
-    </row>
-    <row r="114" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="114" spans="1:22" ht="13.5" customHeight="1">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
+      <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -3872,12 +3703,11 @@
       <c r="T114" s="2"/>
       <c r="U114" s="2"/>
       <c r="V114" s="2"/>
-      <c r="W114" s="2"/>
-    </row>
-    <row r="115" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="115" spans="1:22" ht="13.5" customHeight="1">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
+      <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -3897,12 +3727,11 @@
       <c r="T115" s="2"/>
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
-      <c r="W115" s="2"/>
-    </row>
-    <row r="116" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="116" spans="1:22" ht="13.5" customHeight="1">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
+      <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -3922,12 +3751,11 @@
       <c r="T116" s="2"/>
       <c r="U116" s="2"/>
       <c r="V116" s="2"/>
-      <c r="W116" s="2"/>
-    </row>
-    <row r="117" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="117" spans="1:22" ht="13.5" customHeight="1">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
+      <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -3947,12 +3775,11 @@
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
       <c r="V117" s="2"/>
-      <c r="W117" s="2"/>
-    </row>
-    <row r="118" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="118" spans="1:22" ht="13.5" customHeight="1">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
+      <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -3972,12 +3799,11 @@
       <c r="T118" s="2"/>
       <c r="U118" s="2"/>
       <c r="V118" s="2"/>
-      <c r="W118" s="2"/>
-    </row>
-    <row r="119" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="119" spans="1:22" ht="13.5" customHeight="1">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
+      <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -3997,12 +3823,11 @@
       <c r="T119" s="2"/>
       <c r="U119" s="2"/>
       <c r="V119" s="2"/>
-      <c r="W119" s="2"/>
-    </row>
-    <row r="120" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="120" spans="1:22" ht="13.5" customHeight="1">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
+      <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -4022,12 +3847,11 @@
       <c r="T120" s="2"/>
       <c r="U120" s="2"/>
       <c r="V120" s="2"/>
-      <c r="W120" s="2"/>
-    </row>
-    <row r="121" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="121" spans="1:22" ht="13.5" customHeight="1">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
+      <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -4047,12 +3871,11 @@
       <c r="T121" s="2"/>
       <c r="U121" s="2"/>
       <c r="V121" s="2"/>
-      <c r="W121" s="2"/>
-    </row>
-    <row r="122" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="122" spans="1:22" ht="13.5" customHeight="1">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
+      <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -4072,12 +3895,11 @@
       <c r="T122" s="2"/>
       <c r="U122" s="2"/>
       <c r="V122" s="2"/>
-      <c r="W122" s="2"/>
-    </row>
-    <row r="123" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="123" spans="1:22" ht="13.5" customHeight="1">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
+      <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -4097,12 +3919,11 @@
       <c r="T123" s="2"/>
       <c r="U123" s="2"/>
       <c r="V123" s="2"/>
-      <c r="W123" s="2"/>
-    </row>
-    <row r="124" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="124" spans="1:22" ht="13.5" customHeight="1">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
+      <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -4122,12 +3943,11 @@
       <c r="T124" s="2"/>
       <c r="U124" s="2"/>
       <c r="V124" s="2"/>
-      <c r="W124" s="2"/>
-    </row>
-    <row r="125" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="125" spans="1:22" ht="13.5" customHeight="1">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
+      <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -4147,12 +3967,11 @@
       <c r="T125" s="2"/>
       <c r="U125" s="2"/>
       <c r="V125" s="2"/>
-      <c r="W125" s="2"/>
-    </row>
-    <row r="126" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="126" spans="1:22" ht="13.5" customHeight="1">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
+      <c r="C126" s="2"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -4172,12 +3991,11 @@
       <c r="T126" s="2"/>
       <c r="U126" s="2"/>
       <c r="V126" s="2"/>
-      <c r="W126" s="2"/>
-    </row>
-    <row r="127" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="127" spans="1:22" ht="13.5" customHeight="1">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
-      <c r="C127" s="4"/>
+      <c r="C127" s="2"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
@@ -4197,12 +4015,11 @@
       <c r="T127" s="2"/>
       <c r="U127" s="2"/>
       <c r="V127" s="2"/>
-      <c r="W127" s="2"/>
-    </row>
-    <row r="128" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="128" spans="1:22" ht="13.5" customHeight="1">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
-      <c r="C128" s="4"/>
+      <c r="C128" s="2"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
@@ -4222,12 +4039,11 @@
       <c r="T128" s="2"/>
       <c r="U128" s="2"/>
       <c r="V128" s="2"/>
-      <c r="W128" s="2"/>
-    </row>
-    <row r="129" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="129" spans="1:22" ht="13.5" customHeight="1">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
-      <c r="C129" s="4"/>
+      <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
@@ -4247,12 +4063,11 @@
       <c r="T129" s="2"/>
       <c r="U129" s="2"/>
       <c r="V129" s="2"/>
-      <c r="W129" s="2"/>
-    </row>
-    <row r="130" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="130" spans="1:22" ht="13.5" customHeight="1">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
-      <c r="C130" s="4"/>
+      <c r="C130" s="2"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
@@ -4272,12 +4087,11 @@
       <c r="T130" s="2"/>
       <c r="U130" s="2"/>
       <c r="V130" s="2"/>
-      <c r="W130" s="2"/>
-    </row>
-    <row r="131" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="131" spans="1:22" ht="13.5" customHeight="1">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
-      <c r="C131" s="4"/>
+      <c r="C131" s="2"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
@@ -4297,12 +4111,11 @@
       <c r="T131" s="2"/>
       <c r="U131" s="2"/>
       <c r="V131" s="2"/>
-      <c r="W131" s="2"/>
-    </row>
-    <row r="132" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="132" spans="1:22" ht="13.5" customHeight="1">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
+      <c r="C132" s="2"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
@@ -4322,12 +4135,11 @@
       <c r="T132" s="2"/>
       <c r="U132" s="2"/>
       <c r="V132" s="2"/>
-      <c r="W132" s="2"/>
-    </row>
-    <row r="133" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="133" spans="1:22" ht="13.5" customHeight="1">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
-      <c r="C133" s="4"/>
+      <c r="C133" s="2"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
@@ -4347,12 +4159,11 @@
       <c r="T133" s="2"/>
       <c r="U133" s="2"/>
       <c r="V133" s="2"/>
-      <c r="W133" s="2"/>
-    </row>
-    <row r="134" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="134" spans="1:22" ht="13.5" customHeight="1">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
+      <c r="C134" s="2"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
@@ -4372,12 +4183,11 @@
       <c r="T134" s="2"/>
       <c r="U134" s="2"/>
       <c r="V134" s="2"/>
-      <c r="W134" s="2"/>
-    </row>
-    <row r="135" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="135" spans="1:22" ht="13.5" customHeight="1">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
+      <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -4397,12 +4207,11 @@
       <c r="T135" s="2"/>
       <c r="U135" s="2"/>
       <c r="V135" s="2"/>
-      <c r="W135" s="2"/>
-    </row>
-    <row r="136" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="136" spans="1:22" ht="13.5" customHeight="1">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
-      <c r="C136" s="4"/>
+      <c r="C136" s="2"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
@@ -4422,12 +4231,11 @@
       <c r="T136" s="2"/>
       <c r="U136" s="2"/>
       <c r="V136" s="2"/>
-      <c r="W136" s="2"/>
-    </row>
-    <row r="137" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="137" spans="1:22" ht="13.5" customHeight="1">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
-      <c r="C137" s="4"/>
+      <c r="C137" s="2"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
@@ -4447,12 +4255,11 @@
       <c r="T137" s="2"/>
       <c r="U137" s="2"/>
       <c r="V137" s="2"/>
-      <c r="W137" s="2"/>
-    </row>
-    <row r="138" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="138" spans="1:22" ht="13.5" customHeight="1">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
+      <c r="C138" s="2"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
@@ -4472,12 +4279,11 @@
       <c r="T138" s="2"/>
       <c r="U138" s="2"/>
       <c r="V138" s="2"/>
-      <c r="W138" s="2"/>
-    </row>
-    <row r="139" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="139" spans="1:22" ht="13.5" customHeight="1">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
+      <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
@@ -4497,12 +4303,11 @@
       <c r="T139" s="2"/>
       <c r="U139" s="2"/>
       <c r="V139" s="2"/>
-      <c r="W139" s="2"/>
-    </row>
-    <row r="140" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="140" spans="1:22" ht="13.5" customHeight="1">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
+      <c r="C140" s="2"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
@@ -4522,12 +4327,11 @@
       <c r="T140" s="2"/>
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
-      <c r="W140" s="2"/>
-    </row>
-    <row r="141" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="141" spans="1:22" ht="13.5" customHeight="1">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
+      <c r="C141" s="2"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
@@ -4547,12 +4351,11 @@
       <c r="T141" s="2"/>
       <c r="U141" s="2"/>
       <c r="V141" s="2"/>
-      <c r="W141" s="2"/>
-    </row>
-    <row r="142" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="142" spans="1:22" ht="13.5" customHeight="1">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
-      <c r="C142" s="4"/>
+      <c r="C142" s="2"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
@@ -4572,12 +4375,11 @@
       <c r="T142" s="2"/>
       <c r="U142" s="2"/>
       <c r="V142" s="2"/>
-      <c r="W142" s="2"/>
-    </row>
-    <row r="143" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="143" spans="1:22" ht="13.5" customHeight="1">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
+      <c r="C143" s="2"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
@@ -4597,12 +4399,11 @@
       <c r="T143" s="2"/>
       <c r="U143" s="2"/>
       <c r="V143" s="2"/>
-      <c r="W143" s="2"/>
-    </row>
-    <row r="144" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="144" spans="1:22" ht="13.5" customHeight="1">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
-      <c r="C144" s="4"/>
+      <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
@@ -4622,12 +4423,11 @@
       <c r="T144" s="2"/>
       <c r="U144" s="2"/>
       <c r="V144" s="2"/>
-      <c r="W144" s="2"/>
-    </row>
-    <row r="145" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="145" spans="1:22" ht="13.5" customHeight="1">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
-      <c r="C145" s="4"/>
+      <c r="C145" s="2"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
@@ -4647,12 +4447,11 @@
       <c r="T145" s="2"/>
       <c r="U145" s="2"/>
       <c r="V145" s="2"/>
-      <c r="W145" s="2"/>
-    </row>
-    <row r="146" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="146" spans="1:22" ht="13.5" customHeight="1">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
+      <c r="C146" s="2"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
@@ -4672,12 +4471,11 @@
       <c r="T146" s="2"/>
       <c r="U146" s="2"/>
       <c r="V146" s="2"/>
-      <c r="W146" s="2"/>
-    </row>
-    <row r="147" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="147" spans="1:22" ht="13.5" customHeight="1">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
-      <c r="C147" s="4"/>
+      <c r="C147" s="2"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
@@ -4697,12 +4495,11 @@
       <c r="T147" s="2"/>
       <c r="U147" s="2"/>
       <c r="V147" s="2"/>
-      <c r="W147" s="2"/>
-    </row>
-    <row r="148" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="148" spans="1:22" ht="13.5" customHeight="1">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
-      <c r="C148" s="4"/>
+      <c r="C148" s="2"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
@@ -4722,12 +4519,11 @@
       <c r="T148" s="2"/>
       <c r="U148" s="2"/>
       <c r="V148" s="2"/>
-      <c r="W148" s="2"/>
-    </row>
-    <row r="149" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="149" spans="1:22" ht="13.5" customHeight="1">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
+      <c r="C149" s="2"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
@@ -4747,12 +4543,11 @@
       <c r="T149" s="2"/>
       <c r="U149" s="2"/>
       <c r="V149" s="2"/>
-      <c r="W149" s="2"/>
-    </row>
-    <row r="150" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="150" spans="1:22" ht="13.5" customHeight="1">
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
+      <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
@@ -4772,12 +4567,11 @@
       <c r="T150" s="2"/>
       <c r="U150" s="2"/>
       <c r="V150" s="2"/>
-      <c r="W150" s="2"/>
-    </row>
-    <row r="151" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="151" spans="1:22" ht="13.5" customHeight="1">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
+      <c r="C151" s="2"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
@@ -4797,12 +4591,11 @@
       <c r="T151" s="2"/>
       <c r="U151" s="2"/>
       <c r="V151" s="2"/>
-      <c r="W151" s="2"/>
-    </row>
-    <row r="152" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="152" spans="1:22" ht="13.5" customHeight="1">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
+      <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
@@ -4822,12 +4615,11 @@
       <c r="T152" s="2"/>
       <c r="U152" s="2"/>
       <c r="V152" s="2"/>
-      <c r="W152" s="2"/>
-    </row>
-    <row r="153" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="153" spans="1:22" ht="13.5" customHeight="1">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
+      <c r="C153" s="2"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
@@ -4847,12 +4639,11 @@
       <c r="T153" s="2"/>
       <c r="U153" s="2"/>
       <c r="V153" s="2"/>
-      <c r="W153" s="2"/>
-    </row>
-    <row r="154" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="154" spans="1:22" ht="13.5" customHeight="1">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
-      <c r="C154" s="4"/>
+      <c r="C154" s="2"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
@@ -4872,12 +4663,11 @@
       <c r="T154" s="2"/>
       <c r="U154" s="2"/>
       <c r="V154" s="2"/>
-      <c r="W154" s="2"/>
-    </row>
-    <row r="155" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="155" spans="1:22" ht="13.5" customHeight="1">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
-      <c r="C155" s="4"/>
+      <c r="C155" s="2"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
@@ -4897,12 +4687,11 @@
       <c r="T155" s="2"/>
       <c r="U155" s="2"/>
       <c r="V155" s="2"/>
-      <c r="W155" s="2"/>
-    </row>
-    <row r="156" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="156" spans="1:22" ht="13.5" customHeight="1">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
-      <c r="C156" s="4"/>
+      <c r="C156" s="2"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
@@ -4922,12 +4711,11 @@
       <c r="T156" s="2"/>
       <c r="U156" s="2"/>
       <c r="V156" s="2"/>
-      <c r="W156" s="2"/>
-    </row>
-    <row r="157" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="157" spans="1:22" ht="13.5" customHeight="1">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
-      <c r="C157" s="4"/>
+      <c r="C157" s="2"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
@@ -4947,12 +4735,11 @@
       <c r="T157" s="2"/>
       <c r="U157" s="2"/>
       <c r="V157" s="2"/>
-      <c r="W157" s="2"/>
-    </row>
-    <row r="158" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="158" spans="1:22" ht="13.5" customHeight="1">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
-      <c r="C158" s="4"/>
+      <c r="C158" s="2"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -4972,12 +4759,11 @@
       <c r="T158" s="2"/>
       <c r="U158" s="2"/>
       <c r="V158" s="2"/>
-      <c r="W158" s="2"/>
-    </row>
-    <row r="159" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="159" spans="1:22" ht="13.5" customHeight="1">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
+      <c r="C159" s="2"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
@@ -4997,12 +4783,11 @@
       <c r="T159" s="2"/>
       <c r="U159" s="2"/>
       <c r="V159" s="2"/>
-      <c r="W159" s="2"/>
-    </row>
-    <row r="160" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="160" spans="1:22" ht="13.5" customHeight="1">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
-      <c r="C160" s="4"/>
+      <c r="C160" s="2"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
@@ -5022,12 +4807,11 @@
       <c r="T160" s="2"/>
       <c r="U160" s="2"/>
       <c r="V160" s="2"/>
-      <c r="W160" s="2"/>
-    </row>
-    <row r="161" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="161" spans="1:22" ht="13.5" customHeight="1">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
-      <c r="C161" s="4"/>
+      <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
@@ -5047,12 +4831,11 @@
       <c r="T161" s="2"/>
       <c r="U161" s="2"/>
       <c r="V161" s="2"/>
-      <c r="W161" s="2"/>
-    </row>
-    <row r="162" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="162" spans="1:22" ht="13.5" customHeight="1">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
-      <c r="C162" s="4"/>
+      <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
@@ -5072,12 +4855,11 @@
       <c r="T162" s="2"/>
       <c r="U162" s="2"/>
       <c r="V162" s="2"/>
-      <c r="W162" s="2"/>
-    </row>
-    <row r="163" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="163" spans="1:22" ht="13.5" customHeight="1">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
-      <c r="C163" s="4"/>
+      <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
@@ -5097,12 +4879,11 @@
       <c r="T163" s="2"/>
       <c r="U163" s="2"/>
       <c r="V163" s="2"/>
-      <c r="W163" s="2"/>
-    </row>
-    <row r="164" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="164" spans="1:22" ht="13.5" customHeight="1">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
-      <c r="C164" s="4"/>
+      <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
@@ -5122,12 +4903,11 @@
       <c r="T164" s="2"/>
       <c r="U164" s="2"/>
       <c r="V164" s="2"/>
-      <c r="W164" s="2"/>
-    </row>
-    <row r="165" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="165" spans="1:22" ht="13.5" customHeight="1">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
-      <c r="C165" s="4"/>
+      <c r="C165" s="2"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
@@ -5147,12 +4927,11 @@
       <c r="T165" s="2"/>
       <c r="U165" s="2"/>
       <c r="V165" s="2"/>
-      <c r="W165" s="2"/>
-    </row>
-    <row r="166" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="166" spans="1:22" ht="13.5" customHeight="1">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
-      <c r="C166" s="4"/>
+      <c r="C166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
@@ -5172,12 +4951,11 @@
       <c r="T166" s="2"/>
       <c r="U166" s="2"/>
       <c r="V166" s="2"/>
-      <c r="W166" s="2"/>
-    </row>
-    <row r="167" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="167" spans="1:22" ht="13.5" customHeight="1">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
-      <c r="C167" s="4"/>
+      <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
@@ -5197,12 +4975,11 @@
       <c r="T167" s="2"/>
       <c r="U167" s="2"/>
       <c r="V167" s="2"/>
-      <c r="W167" s="2"/>
-    </row>
-    <row r="168" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="168" spans="1:22" ht="13.5" customHeight="1">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
-      <c r="C168" s="4"/>
+      <c r="C168" s="2"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
@@ -5222,12 +4999,11 @@
       <c r="T168" s="2"/>
       <c r="U168" s="2"/>
       <c r="V168" s="2"/>
-      <c r="W168" s="2"/>
-    </row>
-    <row r="169" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="169" spans="1:22" ht="13.5" customHeight="1">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
-      <c r="C169" s="4"/>
+      <c r="C169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
@@ -5247,12 +5023,11 @@
       <c r="T169" s="2"/>
       <c r="U169" s="2"/>
       <c r="V169" s="2"/>
-      <c r="W169" s="2"/>
-    </row>
-    <row r="170" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="170" spans="1:22" ht="13.5" customHeight="1">
       <c r="A170" s="4"/>
       <c r="B170" s="4"/>
-      <c r="C170" s="4"/>
+      <c r="C170" s="2"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
@@ -5272,12 +5047,11 @@
       <c r="T170" s="2"/>
       <c r="U170" s="2"/>
       <c r="V170" s="2"/>
-      <c r="W170" s="2"/>
-    </row>
-    <row r="171" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="171" spans="1:22" ht="13.5" customHeight="1">
       <c r="A171" s="4"/>
       <c r="B171" s="4"/>
-      <c r="C171" s="4"/>
+      <c r="C171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
@@ -5297,12 +5071,11 @@
       <c r="T171" s="2"/>
       <c r="U171" s="2"/>
       <c r="V171" s="2"/>
-      <c r="W171" s="2"/>
-    </row>
-    <row r="172" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="172" spans="1:22" ht="13.5" customHeight="1">
       <c r="A172" s="4"/>
       <c r="B172" s="4"/>
-      <c r="C172" s="4"/>
+      <c r="C172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
@@ -5322,12 +5095,11 @@
       <c r="T172" s="2"/>
       <c r="U172" s="2"/>
       <c r="V172" s="2"/>
-      <c r="W172" s="2"/>
-    </row>
-    <row r="173" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="173" spans="1:22" ht="13.5" customHeight="1">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
+      <c r="C173" s="2"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
@@ -5347,12 +5119,11 @@
       <c r="T173" s="2"/>
       <c r="U173" s="2"/>
       <c r="V173" s="2"/>
-      <c r="W173" s="2"/>
-    </row>
-    <row r="174" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="174" spans="1:22" ht="13.5" customHeight="1">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
-      <c r="C174" s="3"/>
+      <c r="C174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
@@ -5372,12 +5143,11 @@
       <c r="T174" s="2"/>
       <c r="U174" s="2"/>
       <c r="V174" s="2"/>
-      <c r="W174" s="2"/>
-    </row>
-    <row r="175" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="175" spans="1:22" ht="13.5" customHeight="1">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
-      <c r="C175" s="3"/>
+      <c r="C175" s="2"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
@@ -5397,12 +5167,11 @@
       <c r="T175" s="2"/>
       <c r="U175" s="2"/>
       <c r="V175" s="2"/>
-      <c r="W175" s="2"/>
-    </row>
-    <row r="176" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="176" spans="1:22" ht="13.5" customHeight="1">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
+      <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
@@ -5422,12 +5191,11 @@
       <c r="T176" s="2"/>
       <c r="U176" s="2"/>
       <c r="V176" s="2"/>
-      <c r="W176" s="2"/>
-    </row>
-    <row r="177" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="177" spans="1:22" ht="13.5" customHeight="1">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
-      <c r="C177" s="3"/>
+      <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
@@ -5447,12 +5215,11 @@
       <c r="T177" s="2"/>
       <c r="U177" s="2"/>
       <c r="V177" s="2"/>
-      <c r="W177" s="2"/>
-    </row>
-    <row r="178" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="178" spans="1:22" ht="13.5" customHeight="1">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
-      <c r="C178" s="3"/>
+      <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
@@ -5472,12 +5239,11 @@
       <c r="T178" s="2"/>
       <c r="U178" s="2"/>
       <c r="V178" s="2"/>
-      <c r="W178" s="2"/>
-    </row>
-    <row r="179" spans="1:23" ht="13.5" customHeight="1">
+    </row>
+    <row r="179" spans="1:22" ht="13.5" customHeight="1">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
+      <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
@@ -5497,12 +5263,11 @@
       <c r="T179" s="2"/>
       <c r="U179" s="2"/>
       <c r="V179" s="2"/>
-      <c r="W179" s="2"/>
-    </row>
-    <row r="180" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="180" spans="1:22" ht="15.75" customHeight="1">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
+      <c r="C180" s="6"/>
       <c r="D180" s="6"/>
       <c r="E180" s="6"/>
       <c r="F180" s="6"/>
@@ -5522,12 +5287,11 @@
       <c r="T180" s="6"/>
       <c r="U180" s="6"/>
       <c r="V180" s="6"/>
-      <c r="W180" s="6"/>
-    </row>
-    <row r="181" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="181" spans="1:22" ht="15.75" customHeight="1">
       <c r="A181" s="5"/>
       <c r="B181" s="5"/>
-      <c r="C181" s="5"/>
+      <c r="C181" s="6"/>
       <c r="D181" s="6"/>
       <c r="E181" s="6"/>
       <c r="F181" s="6"/>
@@ -5547,12 +5311,11 @@
       <c r="T181" s="6"/>
       <c r="U181" s="6"/>
       <c r="V181" s="6"/>
-      <c r="W181" s="6"/>
-    </row>
-    <row r="182" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="182" spans="1:22" ht="15.75" customHeight="1">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
-      <c r="C182" s="5"/>
+      <c r="C182" s="6"/>
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
       <c r="F182" s="6"/>
@@ -5572,12 +5335,11 @@
       <c r="T182" s="6"/>
       <c r="U182" s="6"/>
       <c r="V182" s="6"/>
-      <c r="W182" s="6"/>
-    </row>
-    <row r="183" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="183" spans="1:22" ht="15.75" customHeight="1">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
-      <c r="C183" s="5"/>
+      <c r="C183" s="6"/>
       <c r="D183" s="6"/>
       <c r="E183" s="6"/>
       <c r="F183" s="6"/>
@@ -5597,12 +5359,11 @@
       <c r="T183" s="6"/>
       <c r="U183" s="6"/>
       <c r="V183" s="6"/>
-      <c r="W183" s="6"/>
-    </row>
-    <row r="184" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="184" spans="1:22" ht="15.75" customHeight="1">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
-      <c r="C184" s="5"/>
+      <c r="C184" s="6"/>
       <c r="D184" s="6"/>
       <c r="E184" s="6"/>
       <c r="F184" s="6"/>
@@ -5622,12 +5383,11 @@
       <c r="T184" s="6"/>
       <c r="U184" s="6"/>
       <c r="V184" s="6"/>
-      <c r="W184" s="6"/>
-    </row>
-    <row r="185" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="185" spans="1:22" ht="15.75" customHeight="1">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
-      <c r="C185" s="5"/>
+      <c r="C185" s="6"/>
       <c r="D185" s="6"/>
       <c r="E185" s="6"/>
       <c r="F185" s="6"/>
@@ -5647,12 +5407,11 @@
       <c r="T185" s="6"/>
       <c r="U185" s="6"/>
       <c r="V185" s="6"/>
-      <c r="W185" s="6"/>
-    </row>
-    <row r="186" spans="1:23" ht="15.75" customHeight="1">
+    </row>
+    <row r="186" spans="1:22" ht="15.75" customHeight="1">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
-      <c r="C186" s="5"/>
+      <c r="C186" s="6"/>
       <c r="D186" s="6"/>
       <c r="E186" s="6"/>
       <c r="F186" s="6"/>
@@ -5672,14 +5431,13 @@
       <c r="T186" s="6"/>
       <c r="U186" s="6"/>
       <c r="V186" s="6"/>
-      <c r="W186" s="6"/>
-    </row>
-    <row r="187" spans="1:23" ht="15.75" customHeight="1"/>
-    <row r="188" spans="1:23" ht="15.75" customHeight="1"/>
-    <row r="189" spans="1:23" ht="15.75" customHeight="1"/>
-    <row r="190" spans="1:23" ht="15.75" customHeight="1"/>
-    <row r="191" spans="1:23" ht="15.75" customHeight="1"/>
-    <row r="192" spans="1:23" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="187" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="188" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="189" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="190" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="191" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="192" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="193" ht="15.75" customHeight="1"/>
     <row r="194" ht="15.75" customHeight="1"/>
     <row r="195" ht="15.75" customHeight="1"/>
@@ -6315,13 +6073,12 @@
     <row r="825" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{D407A3BE-6ACB-48C4-8CE7-AD8DF5138AA3}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{B217947D-569C-4A46-8ECF-F5D19B5548DC}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{875DD82F-DC20-4E9F-A282-A3CD015B6872}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{77620A62-E017-4775-BB0B-E4DD3A4B4EE2}"/>
-    <hyperlink ref="B56" r:id="rId5" xr:uid="{69F90AE7-C04A-4454-B78C-4ABAA8BB1FB4}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{B217947D-569C-4A46-8ECF-F5D19B5548DC}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{875DD82F-DC20-4E9F-A282-A3CD015B6872}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{77620A62-E017-4775-BB0B-E4DD3A4B4EE2}"/>
+    <hyperlink ref="B56" r:id="rId4" xr:uid="{69F90AE7-C04A-4454-B78C-4ABAA8BB1FB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding screenshot functionality to each step
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ShareWebCopy_Guvi_BestBuy\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56024F-1F63-4964-8547-7D240342898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860C3447-C87F-42AA-B839-9B7CB2CE0AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>KEY</t>
   </si>
@@ -380,17 +380,30 @@
   </si>
   <si>
     <t>Retro Gaming &amp; Arcade;All Video Games;Nintendo Switch 2;ROG Ally Gaming Handheld;Video Game Announcements</t>
+  </si>
+  <si>
+    <t>WRONGPRODUCTNAME</t>
+  </si>
+  <si>
+    <t>!@$$%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -472,31 +485,34 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -717,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V825"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2408,9 +2424,13 @@
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
     </row>
-    <row r="61" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
+    <row r="61" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>121</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -6077,8 +6097,9 @@
     <hyperlink ref="B9" r:id="rId2" xr:uid="{875DD82F-DC20-4E9F-A282-A3CD015B6872}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{77620A62-E017-4775-BB0B-E4DD3A4B4EE2}"/>
     <hyperlink ref="B56" r:id="rId4" xr:uid="{69F90AE7-C04A-4454-B78C-4ABAA8BB1FB4}"/>
+    <hyperlink ref="B61" r:id="rId5" xr:uid="{53DFECD7-AE99-47C2-8D9E-D2ED8D277292}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Chrome Branch Files to Git
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ShareWebCopy_Guvi_BestBuy\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860C3447-C87F-42AA-B839-9B7CB2CE0AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FB6D4-5ED0-4721-91D4-841BB8200002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -731,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V825"/>
+  <dimension ref="A1:V824"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2597,7 +2597,7 @@
       <c r="V67" s="2"/>
     </row>
     <row r="68" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A68" s="9"/>
+      <c r="A68" s="10"/>
       <c r="B68" s="9"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2621,8 +2621,8 @@
       <c r="V68" s="2"/>
     </row>
     <row r="69" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A69" s="10"/>
-      <c r="B69" s="9"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -5093,8 +5093,8 @@
       <c r="V171" s="2"/>
     </row>
     <row r="172" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A172" s="4"/>
-      <c r="B172" s="4"/>
+      <c r="A172" s="3"/>
+      <c r="B172" s="3"/>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
@@ -5260,33 +5260,33 @@
       <c r="U178" s="2"/>
       <c r="V178" s="2"/>
     </row>
-    <row r="179" spans="1:22" ht="13.5" customHeight="1">
+    <row r="179" spans="1:22" ht="15.75" customHeight="1">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
-      <c r="C179" s="2"/>
-      <c r="D179" s="2"/>
-      <c r="E179" s="2"/>
-      <c r="F179" s="2"/>
-      <c r="G179" s="2"/>
-      <c r="H179" s="2"/>
-      <c r="I179" s="2"/>
-      <c r="J179" s="2"/>
-      <c r="K179" s="2"/>
-      <c r="L179" s="2"/>
-      <c r="M179" s="2"/>
-      <c r="N179" s="2"/>
-      <c r="O179" s="2"/>
-      <c r="P179" s="2"/>
-      <c r="Q179" s="2"/>
-      <c r="R179" s="2"/>
-      <c r="S179" s="2"/>
-      <c r="T179" s="2"/>
-      <c r="U179" s="2"/>
-      <c r="V179" s="2"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
+      <c r="I179" s="6"/>
+      <c r="J179" s="6"/>
+      <c r="K179" s="6"/>
+      <c r="L179" s="6"/>
+      <c r="M179" s="6"/>
+      <c r="N179" s="6"/>
+      <c r="O179" s="6"/>
+      <c r="P179" s="6"/>
+      <c r="Q179" s="6"/>
+      <c r="R179" s="6"/>
+      <c r="S179" s="6"/>
+      <c r="T179" s="6"/>
+      <c r="U179" s="6"/>
+      <c r="V179" s="6"/>
     </row>
     <row r="180" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A180" s="3"/>
-      <c r="B180" s="3"/>
+      <c r="A180" s="5"/>
+      <c r="B180" s="5"/>
       <c r="C180" s="6"/>
       <c r="D180" s="6"/>
       <c r="E180" s="6"/>
@@ -5428,30 +5428,7 @@
       <c r="U185" s="6"/>
       <c r="V185" s="6"/>
     </row>
-    <row r="186" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A186" s="5"/>
-      <c r="B186" s="5"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="6"/>
-      <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
-      <c r="G186" s="6"/>
-      <c r="H186" s="6"/>
-      <c r="I186" s="6"/>
-      <c r="J186" s="6"/>
-      <c r="K186" s="6"/>
-      <c r="L186" s="6"/>
-      <c r="M186" s="6"/>
-      <c r="N186" s="6"/>
-      <c r="O186" s="6"/>
-      <c r="P186" s="6"/>
-      <c r="Q186" s="6"/>
-      <c r="R186" s="6"/>
-      <c r="S186" s="6"/>
-      <c r="T186" s="6"/>
-      <c r="U186" s="6"/>
-      <c r="V186" s="6"/>
-    </row>
+    <row r="186" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="187" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="188" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="189" spans="1:22" ht="15.75" customHeight="1"/>
@@ -6090,7 +6067,6 @@
     <row r="822" ht="15.75" customHeight="1"/>
     <row r="823" ht="15.75" customHeight="1"/>
     <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{B217947D-569C-4A46-8ECF-F5D19B5548DC}"/>

</xml_diff>

<commit_message>
Adding Reports,Jenkins and Github files to Git
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ShareWebCopy_Guvi_BestBuy\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FB6D4-5ED0-4721-91D4-841BB8200002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7797377F-7CFF-4EFE-8294-4C9A511C4793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>CTMENUS</t>
   </si>
   <si>
-    <t>Laptops &amp; Desktops;Tablets;Monitors;PC Gaming &amp; Virtual Reality;Computer Components;Hard Drives, SSD &amp; Storage;Computer Accessories;Software;Printers, Ink &amp; Toner;Wi-Fi &amp; Networking;Deals &amp; Outlet;Services &amp; Support;In-Store Experience;</t>
-  </si>
-  <si>
     <t>All Computers &amp; Tablets;Best Buy for Business;Windows Copilot+ PCs;New iPad Pro M4;Google Pixel Tablet</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t>!@$$%</t>
+  </si>
+  <si>
+    <t>Laptops &amp; Desktops;Tablets;Monitors;PC Gaming &amp; Virtual Reality;Computer Components;Hard Drives, SSD &amp; Storage;Computer Accessories;Software;Printers, Ink &amp; Toner;Deals &amp; Outlet;Services &amp; Support;In-Store Experience</t>
   </si>
 </sst>
 </file>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V824"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1166,10 +1166,10 @@
     </row>
     <row r="16" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1253,7 +1253,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1281,7 +1281,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="21" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1334,10 +1334,10 @@
     </row>
     <row r="22" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1362,10 +1362,10 @@
     </row>
     <row r="23" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1390,10 +1390,10 @@
     </row>
     <row r="24" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1418,10 +1418,10 @@
     </row>
     <row r="25" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1446,10 +1446,10 @@
     </row>
     <row r="26" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="27" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1502,10 +1502,10 @@
     </row>
     <row r="28" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1530,10 +1530,10 @@
     </row>
     <row r="29" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="30" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="31" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="32" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="33" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="34" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1698,10 +1698,10 @@
     </row>
     <row r="35" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="36" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="37" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1782,10 +1782,10 @@
     </row>
     <row r="38" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1810,10 +1810,10 @@
     </row>
     <row r="39" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="40" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1866,10 +1866,10 @@
     </row>
     <row r="41" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1894,10 +1894,10 @@
     </row>
     <row r="42" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1922,10 +1922,10 @@
     </row>
     <row r="43" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1950,10 +1950,10 @@
     </row>
     <row r="44" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1978,10 +1978,10 @@
     </row>
     <row r="45" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="46" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="47" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="48" spans="1:22" ht="67.5" customHeight="1" thickBot="1">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2090,10 +2090,10 @@
     </row>
     <row r="49" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2118,10 +2118,10 @@
     </row>
     <row r="50" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2146,10 +2146,10 @@
     </row>
     <row r="51" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2174,10 +2174,10 @@
     </row>
     <row r="52" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A52" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="53" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A53" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2230,10 +2230,10 @@
     </row>
     <row r="54" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A54" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2258,10 +2258,10 @@
     </row>
     <row r="55" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A55" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2286,10 +2286,10 @@
     </row>
     <row r="56" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A56" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2314,10 +2314,10 @@
     </row>
     <row r="57" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2342,10 +2342,10 @@
     </row>
     <row r="58" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A58" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2370,10 +2370,10 @@
     </row>
     <row r="59" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A59" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="60" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2426,10 +2426,10 @@
     </row>
     <row r="61" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
       <c r="A61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="12" t="s">
         <v>120</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>121</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>

</xml_diff>